<commit_message>
corrected fullrun to spikein
</commit_message>
<xml_diff>
--- a/fastqFiles/fastq_12.01.20.xlsx
+++ b/fastqFiles/fastq_12.01.20.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/fastqFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC4737DA-061D-F242-9E57-EDC22CF63059}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA590207-62B3-4C4E-86C4-119DA56FDC2F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3180" yWindow="2020" windowWidth="27640" windowHeight="16940" xr2:uid="{C51EE265-3EF1-2B4E-B3EC-3DAB6702BF9C}"/>
   </bookViews>
@@ -72,9 +72,6 @@
     <t>MidOutput</t>
   </si>
   <si>
-    <t>fullRNASeq</t>
-  </si>
-  <si>
     <t>11.18.20</t>
   </si>
   <si>
@@ -265,6 +262,9 @@
   </si>
   <si>
     <t>Brent_exp30-32_GTAC_32_SIC_Index2_10_AAACCTT_GCTTCTGT_S39_L001_R1_001.fastq.gz</t>
+  </si>
+  <si>
+    <t>spikein</t>
   </si>
 </sst>
 </file>
@@ -627,7 +627,7 @@
   <dimension ref="A1:K63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+      <selection activeCell="G3" sqref="G3:G63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -687,19 +687,19 @@
         <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H2">
         <v>86.1</v>
       </c>
       <c r="I2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J2">
         <v>9678</v>
       </c>
       <c r="K2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -722,19 +722,19 @@
         <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H3">
         <v>90.5</v>
       </c>
       <c r="I3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J3">
         <v>9610</v>
       </c>
       <c r="K3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -757,19 +757,19 @@
         <v>14</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H4">
         <v>133</v>
       </c>
       <c r="I4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J4">
         <v>12498</v>
       </c>
       <c r="K4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -792,19 +792,19 @@
         <v>14</v>
       </c>
       <c r="G5" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H5">
         <v>72.3</v>
       </c>
       <c r="I5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J5">
         <v>11572</v>
       </c>
       <c r="K5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -827,19 +827,19 @@
         <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H6">
         <v>71.900000000000006</v>
       </c>
       <c r="I6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J6">
         <v>11768</v>
       </c>
       <c r="K6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -862,19 +862,19 @@
         <v>14</v>
       </c>
       <c r="G7" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H7">
         <v>31.4</v>
       </c>
       <c r="I7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J7">
         <v>41049</v>
       </c>
       <c r="K7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -897,19 +897,19 @@
         <v>14</v>
       </c>
       <c r="G8" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H8">
         <v>12.1</v>
       </c>
       <c r="I8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J8">
         <v>38416</v>
       </c>
       <c r="K8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -932,19 +932,19 @@
         <v>14</v>
       </c>
       <c r="G9" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H9">
         <v>75.099999999999994</v>
       </c>
       <c r="I9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J9">
         <v>11230</v>
       </c>
       <c r="K9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -967,7 +967,7 @@
         <v>14</v>
       </c>
       <c r="G10" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H10">
         <v>2.04</v>
@@ -979,7 +979,7 @@
         <v>6215</v>
       </c>
       <c r="K10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -1002,19 +1002,19 @@
         <v>14</v>
       </c>
       <c r="G11" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H11">
         <v>10.4</v>
       </c>
       <c r="I11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J11">
         <v>10501</v>
       </c>
       <c r="K11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -1037,19 +1037,19 @@
         <v>14</v>
       </c>
       <c r="G12" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H12">
         <v>170</v>
       </c>
       <c r="I12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J12">
         <v>12636</v>
       </c>
       <c r="K12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -1072,19 +1072,19 @@
         <v>14</v>
       </c>
       <c r="G13" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H13">
         <v>203</v>
       </c>
       <c r="I13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J13">
         <v>12447</v>
       </c>
       <c r="K13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -1107,19 +1107,19 @@
         <v>14</v>
       </c>
       <c r="G14" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H14">
         <v>88.8</v>
       </c>
       <c r="I14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J14">
         <v>12060</v>
       </c>
       <c r="K14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
@@ -1142,19 +1142,19 @@
         <v>14</v>
       </c>
       <c r="G15" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H15">
         <v>72.7</v>
       </c>
       <c r="I15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J15">
         <v>7541</v>
       </c>
       <c r="K15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -1177,19 +1177,19 @@
         <v>14</v>
       </c>
       <c r="G16" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H16">
         <v>127</v>
       </c>
       <c r="I16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J16">
         <v>10818</v>
       </c>
       <c r="K16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
@@ -1212,19 +1212,19 @@
         <v>14</v>
       </c>
       <c r="G17" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H17">
         <v>37.700000000000003</v>
       </c>
       <c r="I17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J17">
         <v>11392</v>
       </c>
       <c r="K17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
@@ -1247,19 +1247,19 @@
         <v>14</v>
       </c>
       <c r="G18" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H18">
         <v>74.900000000000006</v>
       </c>
       <c r="I18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J18">
         <v>10589</v>
       </c>
       <c r="K18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
@@ -1282,7 +1282,7 @@
         <v>14</v>
       </c>
       <c r="G19" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H19">
         <v>0.78600000000000003</v>
@@ -1294,7 +1294,7 @@
         <v>178</v>
       </c>
       <c r="K19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
@@ -1317,19 +1317,19 @@
         <v>14</v>
       </c>
       <c r="G20" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H20">
         <v>175</v>
       </c>
       <c r="I20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J20">
         <v>11860</v>
       </c>
       <c r="K20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
@@ -1352,19 +1352,19 @@
         <v>14</v>
       </c>
       <c r="G21" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H21">
         <v>174</v>
       </c>
       <c r="I21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J21">
         <v>13835</v>
       </c>
       <c r="K21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
@@ -1387,19 +1387,19 @@
         <v>14</v>
       </c>
       <c r="G22" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H22">
         <v>22.7</v>
       </c>
       <c r="I22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J22">
         <v>13623</v>
       </c>
       <c r="K22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
@@ -1422,19 +1422,19 @@
         <v>14</v>
       </c>
       <c r="G23" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H23">
         <v>61.8</v>
       </c>
       <c r="I23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J23">
         <v>10446</v>
       </c>
       <c r="K23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
@@ -1457,19 +1457,19 @@
         <v>14</v>
       </c>
       <c r="G24" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H24">
         <v>30.1</v>
       </c>
       <c r="I24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J24">
         <v>10590</v>
       </c>
       <c r="K24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
@@ -1492,19 +1492,19 @@
         <v>14</v>
       </c>
       <c r="G25" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H25">
         <v>50.1</v>
       </c>
       <c r="I25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J25">
         <v>10328</v>
       </c>
       <c r="K25" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
@@ -1527,19 +1527,19 @@
         <v>14</v>
       </c>
       <c r="G26" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H26">
         <v>75</v>
       </c>
       <c r="I26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J26">
         <v>11889</v>
       </c>
       <c r="K26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
@@ -1562,19 +1562,19 @@
         <v>14</v>
       </c>
       <c r="G27" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H27">
         <v>201</v>
       </c>
       <c r="I27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J27">
         <v>15900</v>
       </c>
       <c r="K27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
@@ -1597,19 +1597,19 @@
         <v>14</v>
       </c>
       <c r="G28" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H28">
         <v>104</v>
       </c>
       <c r="I28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J28">
         <v>11579</v>
       </c>
       <c r="K28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
@@ -1632,19 +1632,19 @@
         <v>14</v>
       </c>
       <c r="G29" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H29">
         <v>154</v>
       </c>
       <c r="I29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J29">
         <v>13035</v>
       </c>
       <c r="K29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
@@ -1667,7 +1667,7 @@
         <v>14</v>
       </c>
       <c r="G30" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H30">
         <v>5</v>
@@ -1679,7 +1679,7 @@
         <v>8313</v>
       </c>
       <c r="K30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
@@ -1702,19 +1702,19 @@
         <v>14</v>
       </c>
       <c r="G31" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H31">
         <v>132</v>
       </c>
       <c r="I31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J31">
         <v>11753</v>
       </c>
       <c r="K31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
@@ -1737,19 +1737,19 @@
         <v>14</v>
       </c>
       <c r="G32" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H32">
         <v>114</v>
       </c>
       <c r="I32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J32">
         <v>12760</v>
       </c>
       <c r="K32" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
@@ -1772,24 +1772,24 @@
         <v>14</v>
       </c>
       <c r="G33" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H33">
         <v>83.5</v>
       </c>
       <c r="I33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J33">
         <v>10569</v>
       </c>
       <c r="K33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B34" t="s">
         <v>12</v>
@@ -1807,7 +1807,7 @@
         <v>14</v>
       </c>
       <c r="G34" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H34">
         <v>1.24</v>
@@ -1819,12 +1819,12 @@
         <v>47250</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B35" t="s">
         <v>12</v>
@@ -1842,24 +1842,24 @@
         <v>14</v>
       </c>
       <c r="G35" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H35">
         <v>44.1</v>
       </c>
       <c r="I35" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J35" s="1">
         <v>9973</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B36" t="s">
         <v>12</v>
@@ -1877,7 +1877,7 @@
         <v>14</v>
       </c>
       <c r="G36" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H36">
         <v>2.42</v>
@@ -1889,12 +1889,12 @@
         <v>11606</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B37" t="s">
         <v>12</v>
@@ -1912,7 +1912,7 @@
         <v>14</v>
       </c>
       <c r="G37" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H37">
         <v>4.76</v>
@@ -1924,12 +1924,12 @@
         <v>9974</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B38" t="s">
         <v>12</v>
@@ -1947,24 +1947,24 @@
         <v>14</v>
       </c>
       <c r="G38" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H38">
         <v>44.43</v>
       </c>
       <c r="I38" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J38" s="1">
         <v>1183</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B39" t="s">
         <v>12</v>
@@ -1982,24 +1982,24 @@
         <v>14</v>
       </c>
       <c r="G39" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H39">
         <v>13</v>
       </c>
       <c r="I39" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J39" s="1">
         <v>12743</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B40" t="s">
         <v>12</v>
@@ -2017,7 +2017,7 @@
         <v>14</v>
       </c>
       <c r="G40" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H40">
         <v>6.4</v>
@@ -2029,12 +2029,12 @@
         <v>12427</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B41" t="s">
         <v>12</v>
@@ -2052,7 +2052,7 @@
         <v>14</v>
       </c>
       <c r="G41" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H41">
         <v>7.19</v>
@@ -2064,12 +2064,12 @@
         <v>11742</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B42" t="s">
         <v>12</v>
@@ -2087,7 +2087,7 @@
         <v>14</v>
       </c>
       <c r="G42" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H42">
         <v>8.52</v>
@@ -2099,12 +2099,12 @@
         <v>10192</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B43" t="s">
         <v>12</v>
@@ -2122,24 +2122,24 @@
         <v>14</v>
       </c>
       <c r="G43" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H43">
         <v>14.5</v>
       </c>
       <c r="I43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J43" s="1">
         <v>11010</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B44" t="s">
         <v>12</v>
@@ -2157,24 +2157,24 @@
         <v>14</v>
       </c>
       <c r="G44" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H44">
         <v>15.2</v>
       </c>
       <c r="I44" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J44" s="1">
         <v>12762</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B45" t="s">
         <v>12</v>
@@ -2192,7 +2192,7 @@
         <v>14</v>
       </c>
       <c r="G45" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H45">
         <v>9.35</v>
@@ -2204,12 +2204,12 @@
         <v>12441</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B46" t="s">
         <v>12</v>
@@ -2227,7 +2227,7 @@
         <v>14</v>
       </c>
       <c r="G46" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H46">
         <v>4.59</v>
@@ -2239,12 +2239,12 @@
         <v>9268</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B47" t="s">
         <v>12</v>
@@ -2262,24 +2262,24 @@
         <v>14</v>
       </c>
       <c r="G47" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H47">
         <v>16.8</v>
       </c>
       <c r="I47" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J47" s="1">
         <v>9759</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B48" t="s">
         <v>12</v>
@@ -2297,24 +2297,24 @@
         <v>14</v>
       </c>
       <c r="G48" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H48">
         <v>12.4</v>
       </c>
       <c r="I48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J48" s="1">
         <v>10725</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B49" t="s">
         <v>12</v>
@@ -2332,24 +2332,24 @@
         <v>14</v>
       </c>
       <c r="G49" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H49">
         <v>18.3</v>
       </c>
       <c r="I49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J49" s="1">
         <v>12194</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B50" t="s">
         <v>12</v>
@@ -2367,24 +2367,24 @@
         <v>14</v>
       </c>
       <c r="G50" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H50">
         <v>21</v>
       </c>
       <c r="I50" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J50" s="1">
         <v>11881</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B51" t="s">
         <v>12</v>
@@ -2402,24 +2402,24 @@
         <v>14</v>
       </c>
       <c r="G51" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H51">
         <v>27.6</v>
       </c>
       <c r="I51" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J51" s="1">
         <v>12836</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B52" t="s">
         <v>12</v>
@@ -2437,24 +2437,24 @@
         <v>14</v>
       </c>
       <c r="G52" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H52">
         <v>12.3</v>
       </c>
       <c r="I52" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J52" s="1">
         <v>12342</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B53" t="s">
         <v>12</v>
@@ -2472,24 +2472,24 @@
         <v>14</v>
       </c>
       <c r="G53" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H53">
         <v>16.100000000000001</v>
       </c>
       <c r="I53" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J53" s="1">
         <v>10750</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B54" t="s">
         <v>12</v>
@@ -2507,7 +2507,7 @@
         <v>14</v>
       </c>
       <c r="G54" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H54">
         <v>6.13</v>
@@ -2519,12 +2519,12 @@
         <v>12846</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B55" t="s">
         <v>12</v>
@@ -2542,7 +2542,7 @@
         <v>14</v>
       </c>
       <c r="G55" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H55">
         <v>3.9</v>
@@ -2554,12 +2554,12 @@
         <v>10643</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B56" t="s">
         <v>12</v>
@@ -2577,7 +2577,7 @@
         <v>14</v>
       </c>
       <c r="G56" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H56">
         <v>2.37</v>
@@ -2589,12 +2589,12 @@
         <v>8588</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B57" t="s">
         <v>12</v>
@@ -2612,7 +2612,7 @@
         <v>14</v>
       </c>
       <c r="G57" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H57">
         <v>0</v>
@@ -2624,12 +2624,12 @@
         <v>561</v>
       </c>
       <c r="K57" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B58" t="s">
         <v>12</v>
@@ -2647,7 +2647,7 @@
         <v>14</v>
       </c>
       <c r="G58" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H58">
         <v>0</v>
@@ -2659,12 +2659,12 @@
         <v>33</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B59" t="s">
         <v>12</v>
@@ -2682,7 +2682,7 @@
         <v>14</v>
       </c>
       <c r="G59" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H59">
         <v>0</v>
@@ -2694,12 +2694,12 @@
         <v>2936</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B60" t="s">
         <v>12</v>
@@ -2717,7 +2717,7 @@
         <v>14</v>
       </c>
       <c r="G60" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H60">
         <v>0</v>
@@ -2729,12 +2729,12 @@
         <v>1989</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B61" t="s">
         <v>12</v>
@@ -2752,7 +2752,7 @@
         <v>14</v>
       </c>
       <c r="G61" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H61">
         <v>3.57</v>
@@ -2764,12 +2764,12 @@
         <v>9858</v>
       </c>
       <c r="K61" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B62" t="s">
         <v>12</v>
@@ -2787,7 +2787,7 @@
         <v>14</v>
       </c>
       <c r="G62" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H62">
         <v>1.63</v>
@@ -2799,12 +2799,12 @@
         <v>10534</v>
       </c>
       <c r="K62" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B63" t="s">
         <v>12</v>
@@ -2822,7 +2822,7 @@
         <v>14</v>
       </c>
       <c r="G63" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="H63">
         <v>0.79100000000000004</v>
@@ -2834,7 +2834,7 @@
         <v>5012</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected 4717 to 4715
</commit_message>
<xml_diff>
--- a/fastqFiles/fastq_12.01.20.xlsx
+++ b/fastqFiles/fastq_12.01.20.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/fastqFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA590207-62B3-4C4E-86C4-119DA56FDC2F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB0AADA-EBBC-DE48-8244-8E23114B6CBB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3180" yWindow="2020" windowWidth="27640" windowHeight="16940" xr2:uid="{C51EE265-3EF1-2B4E-B3EC-3DAB6702BF9C}"/>
   </bookViews>
@@ -627,7 +627,7 @@
   <dimension ref="A1:K63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:G63"/>
+      <selection activeCell="D3" sqref="D3:D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -678,7 +678,7 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E2" t="s">
         <v>13</v>
@@ -713,7 +713,7 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E3" t="s">
         <v>13</v>
@@ -748,7 +748,7 @@
         <v>3</v>
       </c>
       <c r="D4">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>
@@ -783,7 +783,7 @@
         <v>4</v>
       </c>
       <c r="D5">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E5" t="s">
         <v>13</v>
@@ -818,7 +818,7 @@
         <v>5</v>
       </c>
       <c r="D6">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E6" t="s">
         <v>13</v>
@@ -853,7 +853,7 @@
         <v>6</v>
       </c>
       <c r="D7">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E7" t="s">
         <v>13</v>
@@ -888,7 +888,7 @@
         <v>7</v>
       </c>
       <c r="D8">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E8" t="s">
         <v>13</v>
@@ -923,7 +923,7 @@
         <v>8</v>
       </c>
       <c r="D9">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E9" t="s">
         <v>13</v>
@@ -958,7 +958,7 @@
         <v>9</v>
       </c>
       <c r="D10">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E10" t="s">
         <v>13</v>
@@ -993,7 +993,7 @@
         <v>10</v>
       </c>
       <c r="D11">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E11" t="s">
         <v>13</v>
@@ -1028,7 +1028,7 @@
         <v>11</v>
       </c>
       <c r="D12">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E12" t="s">
         <v>13</v>
@@ -1063,7 +1063,7 @@
         <v>12</v>
       </c>
       <c r="D13">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E13" t="s">
         <v>13</v>
@@ -1098,7 +1098,7 @@
         <v>13</v>
       </c>
       <c r="D14">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E14" t="s">
         <v>13</v>
@@ -1133,7 +1133,7 @@
         <v>14</v>
       </c>
       <c r="D15">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E15" t="s">
         <v>13</v>
@@ -1168,7 +1168,7 @@
         <v>15</v>
       </c>
       <c r="D16">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E16" t="s">
         <v>13</v>
@@ -1203,7 +1203,7 @@
         <v>16</v>
       </c>
       <c r="D17">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E17" t="s">
         <v>13</v>
@@ -1238,7 +1238,7 @@
         <v>17</v>
       </c>
       <c r="D18">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E18" t="s">
         <v>13</v>
@@ -1273,7 +1273,7 @@
         <v>18</v>
       </c>
       <c r="D19">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E19" t="s">
         <v>13</v>
@@ -1308,7 +1308,7 @@
         <v>19</v>
       </c>
       <c r="D20">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E20" t="s">
         <v>13</v>
@@ -1343,7 +1343,7 @@
         <v>20</v>
       </c>
       <c r="D21">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E21" t="s">
         <v>13</v>
@@ -1378,7 +1378,7 @@
         <v>21</v>
       </c>
       <c r="D22">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E22" t="s">
         <v>13</v>
@@ -1413,7 +1413,7 @@
         <v>22</v>
       </c>
       <c r="D23">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E23" t="s">
         <v>13</v>
@@ -1448,7 +1448,7 @@
         <v>23</v>
       </c>
       <c r="D24">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E24" t="s">
         <v>13</v>
@@ -1483,7 +1483,7 @@
         <v>24</v>
       </c>
       <c r="D25">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E25" t="s">
         <v>13</v>
@@ -1518,7 +1518,7 @@
         <v>25</v>
       </c>
       <c r="D26">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E26" t="s">
         <v>13</v>
@@ -1553,7 +1553,7 @@
         <v>26</v>
       </c>
       <c r="D27">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E27" t="s">
         <v>13</v>
@@ -1588,7 +1588,7 @@
         <v>27</v>
       </c>
       <c r="D28">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E28" t="s">
         <v>13</v>
@@ -1623,7 +1623,7 @@
         <v>28</v>
       </c>
       <c r="D29">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E29" t="s">
         <v>13</v>
@@ -1658,7 +1658,7 @@
         <v>29</v>
       </c>
       <c r="D30">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E30" t="s">
         <v>13</v>
@@ -1693,7 +1693,7 @@
         <v>30</v>
       </c>
       <c r="D31">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E31" t="s">
         <v>13</v>
@@ -1728,7 +1728,7 @@
         <v>31</v>
       </c>
       <c r="D32">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E32" t="s">
         <v>13</v>
@@ -1763,7 +1763,7 @@
         <v>32</v>
       </c>
       <c r="D33">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E33" t="s">
         <v>13</v>
@@ -1798,7 +1798,7 @@
         <v>1</v>
       </c>
       <c r="D34">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E34" t="s">
         <v>13</v>
@@ -1833,7 +1833,7 @@
         <v>2</v>
       </c>
       <c r="D35">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E35" t="s">
         <v>13</v>
@@ -1868,7 +1868,7 @@
         <v>3</v>
       </c>
       <c r="D36">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E36" t="s">
         <v>13</v>
@@ -1903,7 +1903,7 @@
         <v>4</v>
       </c>
       <c r="D37">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E37" t="s">
         <v>13</v>
@@ -1938,7 +1938,7 @@
         <v>5</v>
       </c>
       <c r="D38">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E38" t="s">
         <v>13</v>
@@ -1973,7 +1973,7 @@
         <v>6</v>
       </c>
       <c r="D39">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E39" t="s">
         <v>13</v>
@@ -2008,7 +2008,7 @@
         <v>7</v>
       </c>
       <c r="D40">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E40" t="s">
         <v>13</v>
@@ -2043,7 +2043,7 @@
         <v>8</v>
       </c>
       <c r="D41">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E41" t="s">
         <v>13</v>
@@ -2078,7 +2078,7 @@
         <v>9</v>
       </c>
       <c r="D42">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E42" t="s">
         <v>13</v>
@@ -2113,7 +2113,7 @@
         <v>10</v>
       </c>
       <c r="D43">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E43" t="s">
         <v>13</v>
@@ -2148,7 +2148,7 @@
         <v>11</v>
       </c>
       <c r="D44">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E44" t="s">
         <v>13</v>
@@ -2183,7 +2183,7 @@
         <v>12</v>
       </c>
       <c r="D45">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E45" t="s">
         <v>13</v>
@@ -2218,7 +2218,7 @@
         <v>13</v>
       </c>
       <c r="D46">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E46" t="s">
         <v>13</v>
@@ -2253,7 +2253,7 @@
         <v>14</v>
       </c>
       <c r="D47">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E47" t="s">
         <v>13</v>
@@ -2288,7 +2288,7 @@
         <v>15</v>
       </c>
       <c r="D48">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E48" t="s">
         <v>13</v>
@@ -2323,7 +2323,7 @@
         <v>16</v>
       </c>
       <c r="D49">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E49" t="s">
         <v>13</v>
@@ -2358,7 +2358,7 @@
         <v>17</v>
       </c>
       <c r="D50">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E50" t="s">
         <v>13</v>
@@ -2393,7 +2393,7 @@
         <v>18</v>
       </c>
       <c r="D51">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E51" t="s">
         <v>13</v>
@@ -2428,7 +2428,7 @@
         <v>19</v>
       </c>
       <c r="D52">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E52" t="s">
         <v>13</v>
@@ -2463,7 +2463,7 @@
         <v>20</v>
       </c>
       <c r="D53">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E53" t="s">
         <v>13</v>
@@ -2498,7 +2498,7 @@
         <v>21</v>
       </c>
       <c r="D54">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E54" t="s">
         <v>13</v>
@@ -2533,7 +2533,7 @@
         <v>22</v>
       </c>
       <c r="D55">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E55" t="s">
         <v>13</v>
@@ -2568,7 +2568,7 @@
         <v>23</v>
       </c>
       <c r="D56">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E56" t="s">
         <v>13</v>
@@ -2603,7 +2603,7 @@
         <v>24</v>
       </c>
       <c r="D57">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E57" t="s">
         <v>13</v>
@@ -2638,7 +2638,7 @@
         <v>25</v>
       </c>
       <c r="D58">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E58" t="s">
         <v>13</v>
@@ -2673,7 +2673,7 @@
         <v>26</v>
       </c>
       <c r="D59">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E59" t="s">
         <v>13</v>
@@ -2708,7 +2708,7 @@
         <v>27</v>
       </c>
       <c r="D60">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E60" t="s">
         <v>13</v>
@@ -2743,7 +2743,7 @@
         <v>28</v>
       </c>
       <c r="D61">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E61" t="s">
         <v>13</v>
@@ -2778,7 +2778,7 @@
         <v>29</v>
       </c>
       <c r="D62">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E62" t="s">
         <v>13</v>
@@ -2813,7 +2813,7 @@
         <v>30</v>
       </c>
       <c r="D63">
-        <v>4717</v>
+        <v>4715</v>
       </c>
       <c r="E63" t="s">
         <v>13</v>

</xml_diff>